<commit_message>
Added excel Driven Implemention
</commit_message>
<xml_diff>
--- a/AutomationPermitPros/TestData/BusinessLicenses.xlsx
+++ b/AutomationPermitPros/TestData/BusinessLicenses.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29704"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_EB55BB073F4D091B71FF0F8EB5DC92488F2776F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7247957D-5DBE-4EB8-8F9A-85C9EDA90B51}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JaganPambala\source\repos\Demo-PermitPros\AutomationPermitPros\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AA8B8D-6C12-4429-9315-6274FCD6A91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BusinessLicense_TestData" sheetId="1" r:id="rId1"/>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="205">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -221,18 +226,9 @@
     <t>Illinois</t>
   </si>
   <si>
-    <t>01/01/2026</t>
-  </si>
-  <si>
     <t>CO</t>
   </si>
   <si>
-    <t>Test license for beer</t>
-  </si>
-  <si>
-    <t>Created via automation</t>
-  </si>
-  <si>
     <t>Delete Testing</t>
   </si>
   <si>
@@ -260,9 +256,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>Certification license</t>
-  </si>
-  <si>
     <t>BL_003</t>
   </si>
   <si>
@@ -651,13 +644,22 @@
   </si>
   <si>
     <t>Report issues through your team's issue tracking system</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>LIC12345678</t>
+  </si>
+  <si>
+    <t>Run</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -693,6 +695,12 @@
       <sz val="12"/>
       <color rgb="FF4472C4"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF6E6E6E"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -754,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -780,10 +788,11 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1086,40 +1095,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH9"/>
+  <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="U3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC18" sqref="AC18"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AG11" sqref="AG11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="6" width="8" customWidth="1"/>
-    <col min="7" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="16" customWidth="1"/>
-    <col min="15" max="16" width="14" customWidth="1"/>
-    <col min="17" max="18" width="20" customWidth="1"/>
-    <col min="19" max="19" width="14" customWidth="1"/>
-    <col min="20" max="20" width="16" customWidth="1"/>
-    <col min="21" max="21" width="20" customWidth="1"/>
-    <col min="22" max="22" width="14" customWidth="1"/>
-    <col min="23" max="24" width="25" customWidth="1"/>
-    <col min="25" max="26" width="15" customWidth="1"/>
-    <col min="27" max="27" width="20" customWidth="1"/>
-    <col min="28" max="29" width="18" customWidth="1"/>
-    <col min="30" max="31" width="15" customWidth="1"/>
-    <col min="32" max="33" width="30" customWidth="1"/>
-    <col min="34" max="34" width="12" customWidth="1"/>
+    <col min="2" max="3" width="18" customWidth="1"/>
+    <col min="4" max="8" width="8" customWidth="1"/>
+    <col min="9" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="16" max="16" width="16" customWidth="1"/>
+    <col min="17" max="18" width="14" customWidth="1"/>
+    <col min="19" max="20" width="20" customWidth="1"/>
+    <col min="21" max="21" width="14" customWidth="1"/>
+    <col min="22" max="22" width="16" customWidth="1"/>
+    <col min="23" max="23" width="20" customWidth="1"/>
+    <col min="24" max="24" width="14" customWidth="1"/>
+    <col min="25" max="26" width="25" customWidth="1"/>
+    <col min="27" max="28" width="15" customWidth="1"/>
+    <col min="29" max="29" width="20" customWidth="1"/>
+    <col min="30" max="31" width="18" customWidth="1"/>
+    <col min="32" max="33" width="15" customWidth="1"/>
+    <col min="34" max="35" width="30" customWidth="1"/>
+    <col min="36" max="36" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:36" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1127,103 +1136,109 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:36" ht="24" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -1243,31 +1258,31 @@
         <v>36</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>37</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>40</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>40</v>
@@ -1279,46 +1294,46 @@
         <v>40</v>
       </c>
       <c r="S2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>51</v>
@@ -1326,174 +1341,188 @@
       <c r="AH2" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:34">
+      <c r="AI2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="N3" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>62</v>
-      </c>
+      <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
-      <c r="V3" s="5" t="s">
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="AD3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE3" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="AF3" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="X3" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="6"/>
-    </row>
-    <row r="4" spans="1:34">
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>54</v>
+      <c r="C4" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>54</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="N4" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="M4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
-      <c r="V4" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="W4" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="X4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6" t="s">
+        <v>71</v>
+      </c>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
-      <c r="AD4" s="6" t="s">
-        <v>67</v>
-      </c>
+      <c r="AD4" s="6"/>
       <c r="AE4" s="6"/>
-      <c r="AF4" s="6"/>
+      <c r="AF4" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="AG4" s="6"/>
       <c r="AH4" s="6"/>
-    </row>
-    <row r="5" spans="1:34">
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
@@ -1510,48 +1539,54 @@
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
       <c r="X5" s="6"/>
-      <c r="Y5" s="6" t="s">
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Z5" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA5" s="6"/>
       <c r="AB5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="AC5" s="6" t="s">
+      <c r="AE5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="AD5" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="6"/>
+      <c r="AF5" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="AG5" s="6"/>
       <c r="AH5" s="6"/>
-    </row>
-    <row r="6" spans="1:34">
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>54</v>
+      <c r="C6" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>53</v>
+      <c r="E6" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="G6" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -1571,41 +1606,47 @@
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
       <c r="AA6" s="6"/>
-      <c r="AB6" s="6" t="s">
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="AC6" s="6" t="s">
+      <c r="AE6" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="AD6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE6" s="6"/>
-      <c r="AF6" s="6"/>
+      <c r="AF6" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="AG6" s="6"/>
       <c r="AH6" s="6"/>
-    </row>
-    <row r="7" spans="1:34">
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="6"/>
+    </row>
+    <row r="7" spans="1:36" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>54</v>
+      <c r="C7" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="G7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="6" t="b">
+        <v>0</v>
+      </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
@@ -1624,135 +1665,147 @@
       <c r="X7" s="6"/>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
-      <c r="AA7" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB7" s="6" t="s">
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="AC7" s="6" t="s">
+      <c r="AE7" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="AD7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE7" s="6"/>
-      <c r="AF7" s="6"/>
+      <c r="AF7" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="AG7" s="6"/>
       <c r="AH7" s="6"/>
-    </row>
-    <row r="8" spans="1:34">
+      <c r="AI7" s="6"/>
+      <c r="AJ7" s="6"/>
+    </row>
+    <row r="8" spans="1:36" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>54</v>
+      <c r="C8" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>54</v>
       </c>
       <c r="G8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>83</v>
-      </c>
       <c r="J8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="L8" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>84</v>
-      </c>
       <c r="M8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="O8" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
-      <c r="V8" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="W8" s="6" t="s">
-        <v>85</v>
-      </c>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
       <c r="X8" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
+        <v>62</v>
+      </c>
+      <c r="Y8" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z8" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
       <c r="AC8" s="6"/>
-      <c r="AD8" s="6" t="s">
-        <v>67</v>
-      </c>
+      <c r="AD8" s="6"/>
       <c r="AE8" s="6"/>
-      <c r="AF8" s="6"/>
+      <c r="AF8" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="AG8" s="6"/>
       <c r="AH8" s="6"/>
-    </row>
-    <row r="9" spans="1:34">
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="6"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="C9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>88</v>
+      <c r="H9" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="I9" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="L9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>90</v>
-      </c>
       <c r="M9" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="O9" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
@@ -1760,48 +1813,54 @@
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
-      <c r="W9" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="X9" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
       <c r="Y9" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z9" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Z9" s="6" t="s">
+      <c r="AB9" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="AA9" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="AB9" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="AC9" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AD9" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE9" s="6"/>
-      <c r="AF9" s="6"/>
+        <v>66</v>
+      </c>
+      <c r="AE9" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF9" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="AG9" s="6"/>
       <c r="AH9" s="6"/>
+      <c r="AI9" s="6"/>
+      <c r="AJ9" s="6"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" errorTitle="Invalid Entry" error="Invalid Module" promptTitle="Module Selection" prompt="Select module type" sqref="B3:B1000" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Business License,Location,Staff Licenses,Dashboard"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorTitle="Invalid Entry" error="Please enter TRUE or FALSE" sqref="C3:C1000 D3:D1000 E3:E1000 F3:F1000" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" errorTitle="Invalid Entry" error="Please enter TRUE or FALSE" sqref="D3:E1000 F3:F1000 G3:G1000 H3:H1000" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="AD3:AD1000" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" sqref="AF3:AF1000" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Pass,Fail,Skip"</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorTitle="Invalid Entry" error="Invalid Module" promptTitle="Module Selection" prompt="Select module type" sqref="C2:C1048576" xr:uid="{EFD8D5E4-5637-451D-B98B-CCB05880B8EC}">
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -1809,19 +1868,19 @@
           <x14:formula1>
             <xm:f>ValidationLists!$C$2:$C$9</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I1000</xm:sqref>
+          <xm:sqref>K3:K1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" errorTitle="Invalid State" error="Select from the list" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>ValidationLists!$E$2:$E$6</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M1000</xm:sqref>
+          <xm:sqref>O3:O1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" errorTitle="Invalid Field" error="Select field to edit" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>ValidationLists!$I$2:$I$10</xm:f>
           </x14:formula1>
-          <xm:sqref>Y3:Y1000</xm:sqref>
+          <xm:sqref>AA3:AA1000</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1833,9 +1892,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
@@ -1844,24 +1905,24 @@
     <col min="9" max="9" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1878,15 +1939,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G3" t="s">
         <v>54</v>
@@ -1895,70 +1956,70 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I10" t="s">
         <v>23</v>
       </c>
@@ -1974,561 +2035,561 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="13"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="12"/>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="7" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="B4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B48" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="9" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="9" t="s">
+    <row r="57" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="9" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="B53" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="B54" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="B55" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="9" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="B58" t="s">
+    <row r="63" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="9" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="B59" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B64" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="B60" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="B61" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="9" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
-      <c r="B64" t="s">
+    <row r="69" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A69" s="9" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="B65" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="B66" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="B67" t="s">
+    <row r="73" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="9" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="9" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
-      <c r="B70" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B75" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
-      <c r="B71" t="s">
+    <row r="78" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A78" s="9" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="9" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B79" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
-      <c r="B74" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
-      <c r="B75" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="B76" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B81" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="9" t="s">
+    <row r="83" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A83" s="9" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
-      <c r="B79" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" s="7" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="B80" t="s">
+      <c r="B84" s="8" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="B81" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" s="7" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="9" t="s">
+      <c r="B85" s="8" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="7" t="s">
+    <row r="86" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A86" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="B86" s="8" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="7" t="s">
+    <row r="87" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A87" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="B85" s="8" t="s">
+      <c r="B87" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="7" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="B88" s="8" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="7" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="B87" s="8" t="s">
+      <c r="B89" s="8" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="7" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B88" s="8" t="s">
+      <c r="B90" s="8" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="7" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B89" s="8" t="s">
+      <c r="B91" s="8" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="7" t="s">
+    <row r="93" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A93" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="B90" s="8" t="s">
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" s="7" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="7" t="s">
+      <c r="B94" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="B91" s="8" t="s">
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" s="7" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="9" t="s">
+      <c r="B95" s="8" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="7" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B94" s="8" t="s">
+      <c r="B96" s="8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="7" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B95" s="8" t="s">
+      <c r="B97" s="8" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="7" t="s">
+    <row r="99" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A99" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="B96" s="8" t="s">
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" s="7" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="7" t="s">
+      <c r="B100" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="B97" s="8" t="s">
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" s="7" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" s="9" t="s">
+      <c r="B101" s="8" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="B100" s="8" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
-      <c r="A101" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="B101" s="8" t="s">
-        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>